<commit_message>
dataset adjustment add jam_layanan and book_search
</commit_message>
<xml_diff>
--- a/aaaaa.xlsx
+++ b/aaaaa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rusdi-prototype-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B06F627C-DB39-4DDB-BDCA-08A34EA7A8B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D82D23-DDB6-4EA5-B96B-8DC806BDF7DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="638">
   <si>
     <t>text</t>
   </si>
@@ -1229,13 +1229,718 @@
   </si>
   <si>
     <t>Apakah perpustakaan buka pada hari ini? Jika ya, pukul berapa?</t>
+  </si>
+  <si>
+    <t>Jam berapa perpustakaan mulai buka hari ini?</t>
+  </si>
+  <si>
+    <t>Perpustakaannya buka dari jam berapa sampai jam berapa?</t>
+  </si>
+  <si>
+    <t>Kapan saja jadwal operasional perpustakaan?</t>
+  </si>
+  <si>
+    <t>Ada info jam layanan perpustakaan nggak?</t>
+  </si>
+  <si>
+    <t>Boleh tahu jam kerja perpustakaan setiap harinya?</t>
+  </si>
+  <si>
+    <t>Hari ini perpustakaan buka sampai jam berapa ya?</t>
+  </si>
+  <si>
+    <t>Saya mau cek jadwal buka perpustakaan.</t>
+  </si>
+  <si>
+    <t>Jam operasional perpustakaan untuk minggu ini bagaimana?</t>
+  </si>
+  <si>
+    <t>Kapan perpustakaan mulai melayani pengunjung?</t>
+  </si>
+  <si>
+    <t>Apakah perpustakaan sudah buka pagi ini?</t>
+  </si>
+  <si>
+    <t>Bisa dibantu dengan informasi jadwal buka perpustakaan?</t>
+  </si>
+  <si>
+    <t>Kapan jam tutup perpustakaan?</t>
+  </si>
+  <si>
+    <t>Jadwal pelayanan perpustakaan harian itu gimana ya?</t>
+  </si>
+  <si>
+    <t>Library-nya hari ini buka jam berapa?</t>
+  </si>
+  <si>
+    <t>Apa aja jam buka dan jam tutupnya tiap hari?</t>
+  </si>
+  <si>
+    <t>Saya ingin tahu jam operasional perpustakaan lengkap satu minggu.</t>
+  </si>
+  <si>
+    <t>Perpustakaan hari ini tutup nggak?</t>
+  </si>
+  <si>
+    <t>Perpustakaan beroperasi dari pukul berapa ke pukul berapa?</t>
+  </si>
+  <si>
+    <t>Tolong informasikan jam layanan hari ini.</t>
+  </si>
+  <si>
+    <t>Jam layanan perpustakaan dimulai pukul berapa?</t>
+  </si>
+  <si>
+    <t>Apakah sekarang perpustakaan sudah buka?</t>
+  </si>
+  <si>
+    <t>Info buka/tutup perpustakaan, dong.</t>
+  </si>
+  <si>
+    <t>Jam berapa perpustakaan mulai dan berhenti melayani?</t>
+  </si>
+  <si>
+    <t>Boleh minta jadwal operasional perpustakaan?</t>
+  </si>
+  <si>
+    <t>Perpustakaan libur hari ini atau tetap buka?</t>
+  </si>
+  <si>
+    <t>Saya ingin tahu kapan bisa mengunjungi perpustakaan.</t>
+  </si>
+  <si>
+    <t>Mohon info jam kerja perpustakaan dari Senin sampai Jumat.</t>
+  </si>
+  <si>
+    <t>Kalau hari Sabtu dan Minggu, perpustakaan buka sampai jam berapa?</t>
+  </si>
+  <si>
+    <t>Kapan perpustakaan tersedia untuk umum?</t>
+  </si>
+  <si>
+    <t>Apakah ada perubahan jam layanan perpustakaan hari ini?</t>
+  </si>
+  <si>
+    <t>Perpus buka jam berapa sih hari ini, Bro?</t>
+  </si>
+  <si>
+    <t>Halo min, perpus udah open belum?</t>
+  </si>
+  <si>
+    <t>Eh, jam operasional perpus tuh dari jam berapa sampe jam berapa sih?</t>
+  </si>
+  <si>
+    <t>Gw pengen main ke perpus, buka ga sih hari ini?</t>
+  </si>
+  <si>
+    <t>Min, info jam bukanya dong, gw mau mampir bentar.</t>
+  </si>
+  <si>
+    <t>Perpusnya buka full day kah hari ini?</t>
+  </si>
+  <si>
+    <t>Hari ini perpus open sampe jam berapa ya?</t>
+  </si>
+  <si>
+    <t>Jam buka-tutup perpus minggu ini gimana, min?</t>
+  </si>
+  <si>
+    <t>Minta rundown jam layanannya dong, biar ga zonk.</t>
+  </si>
+  <si>
+    <t>Ada update ga soal jam buka perpus?</t>
+  </si>
+  <si>
+    <t>Perpusnya libur kah hari ini, atau tetep on?</t>
+  </si>
+  <si>
+    <t>Boleh nanya, perpus standby jam berapa aja?</t>
+  </si>
+  <si>
+    <t>Gw mau ke perpus, jam operasionalnya gimana cuy?</t>
+  </si>
+  <si>
+    <t>Library buka gak siang ini?</t>
+  </si>
+  <si>
+    <t>Min, kalo sorean ke perpus masih buka gak ya?</t>
+  </si>
+  <si>
+    <t>Infoin dong jam kerja perpus yang paling recent.</t>
+  </si>
+  <si>
+    <t>Hari ini perpusnya available jam berapa?</t>
+  </si>
+  <si>
+    <t>Perpus buka tiap hari kah? Atau weekend off?</t>
+  </si>
+  <si>
+    <t>Ada jadwal layanan yang up to date, min?</t>
+  </si>
+  <si>
+    <t>Perpus online jam berapa sampe jam berapa?</t>
+  </si>
+  <si>
+    <t>Jam segini perpus masih buka ga, kira-kira?</t>
+  </si>
+  <si>
+    <t>Eh, perpus start jam berapa kalo weekday?</t>
+  </si>
+  <si>
+    <t>Buka nggak perpusnya pas hari libur gini?</t>
+  </si>
+  <si>
+    <t>Gw pengen numpang baca, bisa dateng jam berapa gitu?</t>
+  </si>
+  <si>
+    <t>Kapan perpus biasanya ready buat pengunjung?</t>
+  </si>
+  <si>
+    <t>Min, kasih tau jam layanannya dong, biar ga kecele.</t>
+  </si>
+  <si>
+    <t>Jam tutupnya biasanya sorean atau malam?</t>
+  </si>
+  <si>
+    <t>Tiap hari jam buka perpus sama terus atau beda-beda?</t>
+  </si>
+  <si>
+    <t>Gw harus dateng pagi ga sih biar dapet tempat?</t>
+  </si>
+  <si>
+    <t>Perpus udah close kah sekarang?</t>
+  </si>
+  <si>
+    <t>Jam buka perpus?</t>
+  </si>
+  <si>
+    <t>Hari ini buka gak?</t>
+  </si>
+  <si>
+    <t>Tutup jam berapa?</t>
+  </si>
+  <si>
+    <t>Perpus open?</t>
+  </si>
+  <si>
+    <t>Jam operasional?</t>
+  </si>
+  <si>
+    <t>Buka dari jam berapa?</t>
+  </si>
+  <si>
+    <t>Sekarang buka gak?</t>
+  </si>
+  <si>
+    <t>Jam layanan?</t>
+  </si>
+  <si>
+    <t>Perpus libur kah?</t>
+  </si>
+  <si>
+    <t>Open jam berapa?</t>
+  </si>
+  <si>
+    <t>Perpus close jam berapa?</t>
+  </si>
+  <si>
+    <t>Hari ini buka?</t>
+  </si>
+  <si>
+    <t>Jadwal buka perpus?</t>
+  </si>
+  <si>
+    <t>Minggu buka gak?</t>
+  </si>
+  <si>
+    <t>Jam berapa mulai?</t>
+  </si>
+  <si>
+    <t>Sekarang masih buka?</t>
+  </si>
+  <si>
+    <t>Jadwal perpus?</t>
+  </si>
+  <si>
+    <t>Tutupnya jam?</t>
+  </si>
+  <si>
+    <t>Kapan buka?</t>
+  </si>
+  <si>
+    <t>Buka gak siang ini?</t>
+  </si>
+  <si>
+    <t>Perpus masih buka?</t>
+  </si>
+  <si>
+    <t>Jam segini buka gak?</t>
+  </si>
+  <si>
+    <t>Malem buka gak?</t>
+  </si>
+  <si>
+    <t>Buka sampe jam?</t>
+  </si>
+  <si>
+    <t>Perpus online jam berapa?</t>
+  </si>
+  <si>
+    <t>Layanan jam brp?</t>
+  </si>
+  <si>
+    <t>Full day kah?</t>
+  </si>
+  <si>
+    <t>Info jam buka?</t>
+  </si>
+  <si>
+    <t>Buka jam berapa sih?</t>
+  </si>
+  <si>
+    <t>Perpus off gak?</t>
+  </si>
+  <si>
+    <t>woi nigga gw mau ke kampus, buka ga?</t>
+  </si>
+  <si>
+    <t>perpus bipa buka kapan?</t>
+  </si>
+  <si>
+    <t>p, buka gx skrg?</t>
+  </si>
+  <si>
+    <t>coek hari ini perpus bipa aktif?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohon informasi terkait jam operasional perpustakaan stmik bina patria </t>
+  </si>
+  <si>
+    <t>info jam buka perpus bipa</t>
+  </si>
+  <si>
+    <t>ingfo min buka kapan</t>
+  </si>
+  <si>
+    <t>perpus bipa kapan buka njir</t>
+  </si>
+  <si>
+    <t>Jam berapa perpustakaan stmik bina patria mulai buka hari ini?</t>
+  </si>
+  <si>
+    <t>beritahu saya jam buka perpustakaan bipa</t>
+  </si>
+  <si>
+    <t>buka gx</t>
+  </si>
+  <si>
+    <t>info jam buka</t>
+  </si>
+  <si>
+    <t>dah tutup belum?</t>
+  </si>
+  <si>
+    <t>hari senin buka gx?</t>
+  </si>
+  <si>
+    <t>apakah hari minggu perpustakaan bina patria buka?</t>
+  </si>
+  <si>
+    <t>jadwal  buka hari jumat siang ??</t>
+  </si>
+  <si>
+    <t>besok buka?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> perpustakaanya open kah?</t>
+  </si>
+  <si>
+    <t>nanti tutup jam berapa?</t>
+  </si>
+  <si>
+    <t>kapan perpustakaan stmik bina patria ditutup?</t>
+  </si>
+  <si>
+    <t>jam berapa bukanya biasanya?</t>
+  </si>
+  <si>
+    <t>terus tutup sampai jam berapa?</t>
+  </si>
+  <si>
+    <t>weekend libur gak nih perpus bipa?</t>
+  </si>
+  <si>
+    <t>pengen nongkrong pas weekend, buka gx?</t>
+  </si>
+  <si>
+    <t>Saya ingin mencari buku.</t>
+  </si>
+  <si>
+    <t>cari_buku</t>
+  </si>
+  <si>
+    <t>Tolong carikan saya buku.</t>
+  </si>
+  <si>
+    <t>Mau nyari buku, bisa bantu?</t>
+  </si>
+  <si>
+    <t>Saya lagi butuh buku, bantu dong.</t>
+  </si>
+  <si>
+    <t>Bisa bantu cari buku?</t>
+  </si>
+  <si>
+    <t>Cariin buku, dong.</t>
+  </si>
+  <si>
+    <t>Saya perlu cari buku.</t>
+  </si>
+  <si>
+    <t>Ada fitur buat nyari buku gak?</t>
+  </si>
+  <si>
+    <t>Saya pengen nyari buku nih.</t>
+  </si>
+  <si>
+    <t>Lagi cari buku, gimana caranya?</t>
+  </si>
+  <si>
+    <t>Buku bisa dicari lewat sini?</t>
+  </si>
+  <si>
+    <t>Saya mau cari buku lewat sistem ini.</t>
+  </si>
+  <si>
+    <t>Bisa tolong bantuin cari buku?</t>
+  </si>
+  <si>
+    <t>Gimana cara nyari buku di sini?</t>
+  </si>
+  <si>
+    <t>Ada yang bisa bantuin cari buku?</t>
+  </si>
+  <si>
+    <t>Saya butuh bantuan buat nyari buku.</t>
+  </si>
+  <si>
+    <t>Tolong bantu cari buku ya.</t>
+  </si>
+  <si>
+    <t>Saya sedang mencari buku sekarang.</t>
+  </si>
+  <si>
+    <t>Bisa bantu temukan buku?</t>
+  </si>
+  <si>
+    <t>Bisa gak nyari buku lewat sini?</t>
+  </si>
+  <si>
+    <t>Saya ingin akses pencarian buku.</t>
+  </si>
+  <si>
+    <t>Saya ingin gunakan fitur cari buku.</t>
+  </si>
+  <si>
+    <t>Tolong aktifkan pencarian buku.</t>
+  </si>
+  <si>
+    <t>Saya coba cari buku dulu, ya.</t>
+  </si>
+  <si>
+    <t>Boleh cari buku di sini?</t>
+  </si>
+  <si>
+    <t>Ada menu buat cari buku?</t>
+  </si>
+  <si>
+    <t>Minta tolong, saya mau cari buku.</t>
+  </si>
+  <si>
+    <t>Saya pengen akses daftar buku.</t>
+  </si>
+  <si>
+    <t>Lagi nyari buku nih, bisa dibantu?</t>
+  </si>
+  <si>
+    <t>Mau lihat-lihat buku dulu, gimana caranya?</t>
+  </si>
+  <si>
+    <t>Gw mau nyari buku nih.</t>
+  </si>
+  <si>
+    <t>Min, bantuin cari buku dong.</t>
+  </si>
+  <si>
+    <t>Lagi pengen baca, bisa cari buku di sini?</t>
+  </si>
+  <si>
+    <t>Mau cari-cari buku dulu nih.</t>
+  </si>
+  <si>
+    <t>Ada fitur find book di sini gak?</t>
+  </si>
+  <si>
+    <t>Min, cari buku bisa lewat sini ya?</t>
+  </si>
+  <si>
+    <t>Cuy, gw butuh buku nih, help dong.</t>
+  </si>
+  <si>
+    <t>Bisa tolong search-in buku?</t>
+  </si>
+  <si>
+    <t>Cari buku dulu ya, boleh kan?</t>
+  </si>
+  <si>
+    <t>Woy, cariin buku dong 😭</t>
+  </si>
+  <si>
+    <t>Ada menu buat hunting buku nggak?</t>
+  </si>
+  <si>
+    <t>Pengen nyari buku tapi males ribet, ada cara gampang gak?</t>
+  </si>
+  <si>
+    <t>Mau liat-liat buku dulu ah.</t>
+  </si>
+  <si>
+    <t>Bro, bisa bantuin cari buku gak?</t>
+  </si>
+  <si>
+    <t>Perlu buku nih, gimana cara nyarinya?</t>
+  </si>
+  <si>
+    <t>Boleh dong, bantu gw cari buku.</t>
+  </si>
+  <si>
+    <t>Euy, mau baca-baca, cariin buku atuh.</t>
+  </si>
+  <si>
+    <t>Bisa bantu gw track buku ga?</t>
+  </si>
+  <si>
+    <t>Gimana caranya browsing buku di sini?</t>
+  </si>
+  <si>
+    <t>Lagi butuh referensi, cari buku yuk.</t>
+  </si>
+  <si>
+    <t>Ada opsi buat nyari buku gak sih?</t>
+  </si>
+  <si>
+    <t>Mau cek-cek buku dulu nih.</t>
+  </si>
+  <si>
+    <t>Ada search bar buat buku nggak?</t>
+  </si>
+  <si>
+    <t>Min, books search aktif gak?</t>
+  </si>
+  <si>
+    <t>Bang, bantu cari buku ya.</t>
+  </si>
+  <si>
+    <t>Lagi butuh buku buat tugas, bisa bantu cari?</t>
+  </si>
+  <si>
+    <t>Misi, numpang cari buku yak.</t>
+  </si>
+  <si>
+    <t>Woke bentar, cari buku dulu deh.</t>
+  </si>
+  <si>
+    <t>Cari buku yuk, siapa tau nemu yang pas.</t>
+  </si>
+  <si>
+    <t>Min, ada fitur scan buku ga, eh maksudnya cari buku?</t>
+  </si>
+  <si>
+    <t>Cari buku.</t>
+  </si>
+  <si>
+    <t>Nyari buku.</t>
+  </si>
+  <si>
+    <t>Mau buku.</t>
+  </si>
+  <si>
+    <t>Butuh buku.</t>
+  </si>
+  <si>
+    <t>Buku dong.</t>
+  </si>
+  <si>
+    <t>Bisa cari buku?</t>
+  </si>
+  <si>
+    <t>Cariin buku.</t>
+  </si>
+  <si>
+    <t>Pengin buku.</t>
+  </si>
+  <si>
+    <t>Gw cari buku.</t>
+  </si>
+  <si>
+    <t>Buku mana?</t>
+  </si>
+  <si>
+    <t>Buku ada?</t>
+  </si>
+  <si>
+    <t>Buku di mana?</t>
+  </si>
+  <si>
+    <t>Liat buku.</t>
+  </si>
+  <si>
+    <t>Minta buku.</t>
+  </si>
+  <si>
+    <t>Ada buku?</t>
+  </si>
+  <si>
+    <t>Mau liat buku.</t>
+  </si>
+  <si>
+    <t>Pengen liat buku.</t>
+  </si>
+  <si>
+    <t>Akses buku.</t>
+  </si>
+  <si>
+    <t>Buka buku.</t>
+  </si>
+  <si>
+    <t>Search buku.</t>
+  </si>
+  <si>
+    <t>Buku please.</t>
+  </si>
+  <si>
+    <t>Buka list buku.</t>
+  </si>
+  <si>
+    <t>Misi cari buku.</t>
+  </si>
+  <si>
+    <t>Browse buku.</t>
+  </si>
+  <si>
+    <t>Show buku.</t>
+  </si>
+  <si>
+    <t>Temuin buu.</t>
+  </si>
+  <si>
+    <t>Ketik buku.</t>
+  </si>
+  <si>
+    <t>Lacak buku.</t>
+  </si>
+  <si>
+    <t>Cek buku.</t>
+  </si>
+  <si>
+    <t>Scan buku.</t>
+  </si>
+  <si>
+    <t>Saya ingin mencari buku tentang pemrograman.</t>
+  </si>
+  <si>
+    <t>Ada buku jaringan komputer gak?</t>
+  </si>
+  <si>
+    <t>Cariin buku coding dong.</t>
+  </si>
+  <si>
+    <t>Punya buku AI nggak, min?</t>
+  </si>
+  <si>
+    <t>Mau cari buku tentang machine learning.</t>
+  </si>
+  <si>
+    <t>Min, tolong cariin buku basis data.</t>
+  </si>
+  <si>
+    <t>Ada buku pemrograman web?</t>
+  </si>
+  <si>
+    <t>Lagi nyari buku tentang algoritma.</t>
+  </si>
+  <si>
+    <t>Min, buku komputer tersedia nggak?</t>
+  </si>
+  <si>
+    <t>Pengen baca buku seputar keamanan jaringan.</t>
+  </si>
+  <si>
+    <t>Cari buku python, ada gak?</t>
+  </si>
+  <si>
+    <t>Ada rekomendasi buku sistem operasi?</t>
+  </si>
+  <si>
+    <t>Mau liat buku tentang cloud computing.</t>
+  </si>
+  <si>
+    <t>Buku tentang big data ada kah</t>
+  </si>
+  <si>
+    <t>Boleh cari buku pemrograman Java?</t>
+  </si>
+  <si>
+    <t>Ada buku tentang struktur data gak?</t>
+  </si>
+  <si>
+    <t>Min, buku tentang teknologi terbaru di TI ada?</t>
+  </si>
+  <si>
+    <t>Lagi butuh buku buat belajar SQL.</t>
+  </si>
+  <si>
+    <t>Gw pengen cari buku pemrograman dasar.</t>
+  </si>
+  <si>
+    <t>Min, ada buku tentang IoT?</t>
+  </si>
+  <si>
+    <t>Cariin buku tentang blockchain dong.</t>
+  </si>
+  <si>
+    <t>Ada gak buku AI yang pemula friendly?</t>
+  </si>
+  <si>
+    <t>Buku deep learning tersedia?</t>
+  </si>
+  <si>
+    <t>Pengen cari buku programming mobile.</t>
+  </si>
+  <si>
+    <t>Mau cari buku tentang data science.</t>
+  </si>
+  <si>
+    <t>Cariin dong buku keamanan siber.</t>
+  </si>
+  <si>
+    <t>Buku web development yang bagus ada?</t>
+  </si>
+  <si>
+    <t>Lagi nyari buku UI/UX design.</t>
+  </si>
+  <si>
+    <t>Min, saya cari buku tentang analisis sistem.</t>
+  </si>
+  <si>
+    <t>Punya buku tentang rekayasa perangkat lunak?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1366,14 +2071,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1725,7 +2422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2081,78 +2778,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D401"/>
+  <dimension ref="A1:C642"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C1" sqref="C1:D169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="D1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>239</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>240</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>241</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>242</v>
       </c>
@@ -2160,7 +2846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>243</v>
       </c>
@@ -2168,7 +2854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2176,7 +2862,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -2184,7 +2870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>244</v>
       </c>
@@ -2192,7 +2878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>245</v>
       </c>
@@ -2200,7 +2886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2208,7 +2894,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2216,7 +2902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -2224,7 +2910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>246</v>
       </c>
@@ -2232,7 +2918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -5318,6 +6004,1934 @@
       </c>
       <c r="B401" t="s">
         <v>396</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>0</v>
+      </c>
+      <c r="B402" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>398</v>
+      </c>
+      <c r="B403" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>402</v>
+      </c>
+      <c r="B404" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>399</v>
+      </c>
+      <c r="B405" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>400</v>
+      </c>
+      <c r="B406" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>401</v>
+      </c>
+      <c r="B407" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>403</v>
+      </c>
+      <c r="B408" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>433</v>
+      </c>
+      <c r="B409" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>434</v>
+      </c>
+      <c r="B410" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>435</v>
+      </c>
+      <c r="B411" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>436</v>
+      </c>
+      <c r="B412" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>437</v>
+      </c>
+      <c r="B413" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>438</v>
+      </c>
+      <c r="B414" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>439</v>
+      </c>
+      <c r="B415" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>440</v>
+      </c>
+      <c r="B416" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>441</v>
+      </c>
+      <c r="B417" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>442</v>
+      </c>
+      <c r="B418" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>443</v>
+      </c>
+      <c r="B419" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>444</v>
+      </c>
+      <c r="B420" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>445</v>
+      </c>
+      <c r="B421" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>446</v>
+      </c>
+      <c r="B422" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>447</v>
+      </c>
+      <c r="B423" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>448</v>
+      </c>
+      <c r="B424" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>449</v>
+      </c>
+      <c r="B425" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>450</v>
+      </c>
+      <c r="B426" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>451</v>
+      </c>
+      <c r="B427" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>452</v>
+      </c>
+      <c r="B428" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>453</v>
+      </c>
+      <c r="B429" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>454</v>
+      </c>
+      <c r="B430" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>455</v>
+      </c>
+      <c r="B431" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>456</v>
+      </c>
+      <c r="B432" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>457</v>
+      </c>
+      <c r="B433" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>458</v>
+      </c>
+      <c r="B434" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>459</v>
+      </c>
+      <c r="B435" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>460</v>
+      </c>
+      <c r="B436" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>461</v>
+      </c>
+      <c r="B437" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>462</v>
+      </c>
+      <c r="B438" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>403</v>
+      </c>
+      <c r="B439" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>404</v>
+      </c>
+      <c r="B440" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>405</v>
+      </c>
+      <c r="B441" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>406</v>
+      </c>
+      <c r="B442" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>407</v>
+      </c>
+      <c r="B443" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>408</v>
+      </c>
+      <c r="B444" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>409</v>
+      </c>
+      <c r="B445" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>410</v>
+      </c>
+      <c r="B446" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>411</v>
+      </c>
+      <c r="B447" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>412</v>
+      </c>
+      <c r="B448" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>413</v>
+      </c>
+      <c r="B449" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>414</v>
+      </c>
+      <c r="B450" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>415</v>
+      </c>
+      <c r="B451" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>416</v>
+      </c>
+      <c r="B452" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>417</v>
+      </c>
+      <c r="B453" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>418</v>
+      </c>
+      <c r="B454" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>419</v>
+      </c>
+      <c r="B455" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>420</v>
+      </c>
+      <c r="B456" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>421</v>
+      </c>
+      <c r="B457" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>422</v>
+      </c>
+      <c r="B458" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>423</v>
+      </c>
+      <c r="B459" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>424</v>
+      </c>
+      <c r="B460" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>425</v>
+      </c>
+      <c r="B461" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>426</v>
+      </c>
+      <c r="B462" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>427</v>
+      </c>
+      <c r="B463" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>428</v>
+      </c>
+      <c r="B464" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>429</v>
+      </c>
+      <c r="B465" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>430</v>
+      </c>
+      <c r="B466" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>431</v>
+      </c>
+      <c r="B467" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>432</v>
+      </c>
+      <c r="B468" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>463</v>
+      </c>
+      <c r="B469" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>464</v>
+      </c>
+      <c r="B470" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>465</v>
+      </c>
+      <c r="B471" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>466</v>
+      </c>
+      <c r="B472" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>467</v>
+      </c>
+      <c r="B473" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>468</v>
+      </c>
+      <c r="B474" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>469</v>
+      </c>
+      <c r="B475" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>470</v>
+      </c>
+      <c r="B476" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>471</v>
+      </c>
+      <c r="B477" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>472</v>
+      </c>
+      <c r="B478" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>473</v>
+      </c>
+      <c r="B479" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>474</v>
+      </c>
+      <c r="B480" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>475</v>
+      </c>
+      <c r="B481" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>476</v>
+      </c>
+      <c r="B482" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>477</v>
+      </c>
+      <c r="B483" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>478</v>
+      </c>
+      <c r="B484" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>479</v>
+      </c>
+      <c r="B485" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>480</v>
+      </c>
+      <c r="B486" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>481</v>
+      </c>
+      <c r="B487" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>482</v>
+      </c>
+      <c r="B488" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>483</v>
+      </c>
+      <c r="B489" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="490" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>484</v>
+      </c>
+      <c r="B490" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>485</v>
+      </c>
+      <c r="B491" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>486</v>
+      </c>
+      <c r="B492" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>487</v>
+      </c>
+      <c r="B493" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>488</v>
+      </c>
+      <c r="B494" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>489</v>
+      </c>
+      <c r="B495" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>490</v>
+      </c>
+      <c r="B496" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>491</v>
+      </c>
+      <c r="B497" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>492</v>
+      </c>
+      <c r="B498" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>493</v>
+      </c>
+      <c r="B499" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>494</v>
+      </c>
+      <c r="B500" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>495</v>
+      </c>
+      <c r="B501" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="502" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>496</v>
+      </c>
+      <c r="B502" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="503" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>497</v>
+      </c>
+      <c r="B503" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="504" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>498</v>
+      </c>
+      <c r="B504" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="505" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>499</v>
+      </c>
+      <c r="B505" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="506" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>500</v>
+      </c>
+      <c r="B506" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="507" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A507" t="s">
+        <v>501</v>
+      </c>
+      <c r="B507" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="508" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>502</v>
+      </c>
+      <c r="B508" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="509" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>503</v>
+      </c>
+      <c r="B509" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="510" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>504</v>
+      </c>
+      <c r="B510" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="511" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>505</v>
+      </c>
+      <c r="B511" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="512" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>506</v>
+      </c>
+      <c r="B512" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="513" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>507</v>
+      </c>
+      <c r="B513" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="514" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>508</v>
+      </c>
+      <c r="B514" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="515" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>509</v>
+      </c>
+      <c r="B515" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="516" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>510</v>
+      </c>
+      <c r="B516" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="517" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>511</v>
+      </c>
+      <c r="B517" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="518" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>512</v>
+      </c>
+      <c r="B518" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="519" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A519" t="s">
+        <v>513</v>
+      </c>
+      <c r="B519" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="520" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>514</v>
+      </c>
+      <c r="B520" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="521" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A521" t="s">
+        <v>515</v>
+      </c>
+      <c r="B521" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="522" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A522" t="s">
+        <v>516</v>
+      </c>
+      <c r="B522" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="523" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A523" t="s">
+        <v>517</v>
+      </c>
+      <c r="B523" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="524" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A524" t="s">
+        <v>519</v>
+      </c>
+      <c r="B524" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="525" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A525" t="s">
+        <v>520</v>
+      </c>
+      <c r="B525" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="526" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A526" t="s">
+        <v>521</v>
+      </c>
+      <c r="B526" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="527" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A527" t="s">
+        <v>522</v>
+      </c>
+      <c r="B527" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="528" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A528" t="s">
+        <v>523</v>
+      </c>
+      <c r="B528" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="529" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A529" t="s">
+        <v>524</v>
+      </c>
+      <c r="B529" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="530" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A530" t="s">
+        <v>525</v>
+      </c>
+      <c r="B530" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="531" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A531" t="s">
+        <v>526</v>
+      </c>
+      <c r="B531" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="532" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A532" t="s">
+        <v>527</v>
+      </c>
+      <c r="B532" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="533" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A533" t="s">
+        <v>528</v>
+      </c>
+      <c r="B533" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="534" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A534" t="s">
+        <v>529</v>
+      </c>
+      <c r="B534" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="535" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A535" t="s">
+        <v>530</v>
+      </c>
+      <c r="B535" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="536" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A536" t="s">
+        <v>531</v>
+      </c>
+      <c r="B536" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="537" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A537" t="s">
+        <v>532</v>
+      </c>
+      <c r="B537" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="538" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A538" t="s">
+        <v>533</v>
+      </c>
+      <c r="B538" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="539" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A539" t="s">
+        <v>534</v>
+      </c>
+      <c r="B539" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="540" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A540" t="s">
+        <v>535</v>
+      </c>
+      <c r="B540" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="541" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A541" t="s">
+        <v>536</v>
+      </c>
+      <c r="B541" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="542" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A542" t="s">
+        <v>537</v>
+      </c>
+      <c r="B542" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="543" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A543" t="s">
+        <v>538</v>
+      </c>
+      <c r="B543" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="544" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A544" t="s">
+        <v>539</v>
+      </c>
+      <c r="B544" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="545" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A545" t="s">
+        <v>540</v>
+      </c>
+      <c r="B545" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="546" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A546" t="s">
+        <v>541</v>
+      </c>
+      <c r="B546" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="547" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A547" t="s">
+        <v>542</v>
+      </c>
+      <c r="B547" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="548" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A548" t="s">
+        <v>543</v>
+      </c>
+      <c r="B548" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="549" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A549" t="s">
+        <v>544</v>
+      </c>
+      <c r="B549" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="550" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A550" t="s">
+        <v>545</v>
+      </c>
+      <c r="B550" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="551" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A551" t="s">
+        <v>546</v>
+      </c>
+      <c r="B551" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="552" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A552" t="s">
+        <v>547</v>
+      </c>
+      <c r="B552" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="553" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
+        <v>548</v>
+      </c>
+      <c r="B553" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="554" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>549</v>
+      </c>
+      <c r="B554" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="555" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
+        <v>550</v>
+      </c>
+      <c r="B555" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="556" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>551</v>
+      </c>
+      <c r="B556" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="557" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>552</v>
+      </c>
+      <c r="B557" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="558" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A558" t="s">
+        <v>553</v>
+      </c>
+      <c r="B558" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="559" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A559" t="s">
+        <v>554</v>
+      </c>
+      <c r="B559" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="560" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>555</v>
+      </c>
+      <c r="B560" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="561" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>556</v>
+      </c>
+      <c r="B561" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="562" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A562" t="s">
+        <v>557</v>
+      </c>
+      <c r="B562" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="563" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
+        <v>558</v>
+      </c>
+      <c r="B563" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="564" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A564" t="s">
+        <v>559</v>
+      </c>
+      <c r="B564" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="565" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A565" t="s">
+        <v>560</v>
+      </c>
+      <c r="B565" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="566" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>561</v>
+      </c>
+      <c r="B566" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="567" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>562</v>
+      </c>
+      <c r="B567" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="568" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A568" t="s">
+        <v>563</v>
+      </c>
+      <c r="B568" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="569" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>564</v>
+      </c>
+      <c r="B569" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="570" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
+        <v>565</v>
+      </c>
+      <c r="B570" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="571" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
+        <v>566</v>
+      </c>
+      <c r="B571" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="572" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A572" t="s">
+        <v>567</v>
+      </c>
+      <c r="B572" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="573" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A573" t="s">
+        <v>568</v>
+      </c>
+      <c r="B573" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="574" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A574" t="s">
+        <v>569</v>
+      </c>
+      <c r="B574" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="575" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
+        <v>570</v>
+      </c>
+      <c r="B575" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="576" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A576" t="s">
+        <v>571</v>
+      </c>
+      <c r="B576" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="577" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
+        <v>572</v>
+      </c>
+      <c r="B577" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="578" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>573</v>
+      </c>
+      <c r="B578" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="579" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
+        <v>574</v>
+      </c>
+      <c r="B579" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="580" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A580" t="s">
+        <v>575</v>
+      </c>
+      <c r="B580" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="581" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
+        <v>576</v>
+      </c>
+      <c r="B581" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="582" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A582" t="s">
+        <v>577</v>
+      </c>
+      <c r="B582" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="583" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A583" t="s">
+        <v>578</v>
+      </c>
+      <c r="B583" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="584" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A584" t="s">
+        <v>579</v>
+      </c>
+      <c r="B584" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="585" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A585" t="s">
+        <v>580</v>
+      </c>
+      <c r="B585" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="586" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A586" t="s">
+        <v>581</v>
+      </c>
+      <c r="B586" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="587" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A587" t="s">
+        <v>582</v>
+      </c>
+      <c r="B587" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="588" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A588" t="s">
+        <v>583</v>
+      </c>
+      <c r="B588" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="589" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A589" t="s">
+        <v>584</v>
+      </c>
+      <c r="B589" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="590" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A590" t="s">
+        <v>585</v>
+      </c>
+      <c r="B590" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="591" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A591" t="s">
+        <v>586</v>
+      </c>
+      <c r="B591" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="592" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A592" t="s">
+        <v>587</v>
+      </c>
+      <c r="B592" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="593" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A593" t="s">
+        <v>588</v>
+      </c>
+      <c r="B593" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="594" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A594" t="s">
+        <v>589</v>
+      </c>
+      <c r="B594" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="595" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A595" t="s">
+        <v>590</v>
+      </c>
+      <c r="B595" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="596" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A596" t="s">
+        <v>591</v>
+      </c>
+      <c r="B596" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="597" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A597" t="s">
+        <v>592</v>
+      </c>
+      <c r="B597" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="598" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A598" t="s">
+        <v>593</v>
+      </c>
+      <c r="B598" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="599" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A599" t="s">
+        <v>594</v>
+      </c>
+      <c r="B599" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="600" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A600" t="s">
+        <v>595</v>
+      </c>
+      <c r="B600" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="601" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A601" t="s">
+        <v>596</v>
+      </c>
+      <c r="B601" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="602" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>597</v>
+      </c>
+      <c r="B602" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="603" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A603" t="s">
+        <v>598</v>
+      </c>
+      <c r="B603" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="604" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A604" t="s">
+        <v>599</v>
+      </c>
+      <c r="B604" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="605" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A605" t="s">
+        <v>600</v>
+      </c>
+      <c r="B605" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="606" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A606" t="s">
+        <v>601</v>
+      </c>
+      <c r="B606" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="607" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A607" t="s">
+        <v>602</v>
+      </c>
+      <c r="B607" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="608" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A608" t="s">
+        <v>603</v>
+      </c>
+      <c r="B608" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="609" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A609" t="s">
+        <v>604</v>
+      </c>
+      <c r="B609" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="610" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A610" t="s">
+        <v>605</v>
+      </c>
+      <c r="B610" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="611" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A611" t="s">
+        <v>606</v>
+      </c>
+      <c r="B611" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="612" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A612" t="s">
+        <v>607</v>
+      </c>
+      <c r="B612" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="613" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A613" t="s">
+        <v>608</v>
+      </c>
+      <c r="B613" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A614" t="s">
+        <v>609</v>
+      </c>
+      <c r="B614" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="615" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A615" t="s">
+        <v>610</v>
+      </c>
+      <c r="B615" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="616" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A616" t="s">
+        <v>611</v>
+      </c>
+      <c r="B616" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="617" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A617" t="s">
+        <v>612</v>
+      </c>
+      <c r="B617" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="618" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A618" t="s">
+        <v>613</v>
+      </c>
+      <c r="B618" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="619" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A619" t="s">
+        <v>614</v>
+      </c>
+      <c r="B619" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="620" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A620" t="s">
+        <v>615</v>
+      </c>
+      <c r="B620" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="621" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A621" t="s">
+        <v>616</v>
+      </c>
+      <c r="B621" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="622" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A622" t="s">
+        <v>617</v>
+      </c>
+      <c r="B622" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="623" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A623" t="s">
+        <v>618</v>
+      </c>
+      <c r="B623" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="624" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A624" t="s">
+        <v>619</v>
+      </c>
+      <c r="B624" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="625" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A625" t="s">
+        <v>620</v>
+      </c>
+      <c r="B625" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="626" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A626" t="s">
+        <v>621</v>
+      </c>
+      <c r="B626" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="627" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A627" t="s">
+        <v>622</v>
+      </c>
+      <c r="B627" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="628" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A628" t="s">
+        <v>623</v>
+      </c>
+      <c r="B628" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="629" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A629" t="s">
+        <v>624</v>
+      </c>
+      <c r="B629" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="630" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A630" t="s">
+        <v>625</v>
+      </c>
+      <c r="B630" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="631" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A631" t="s">
+        <v>626</v>
+      </c>
+      <c r="B631" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="632" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A632" t="s">
+        <v>627</v>
+      </c>
+      <c r="B632" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="633" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A633" t="s">
+        <v>628</v>
+      </c>
+      <c r="B633" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="634" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A634" t="s">
+        <v>629</v>
+      </c>
+      <c r="B634" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="635" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A635" t="s">
+        <v>630</v>
+      </c>
+      <c r="B635" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="636" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A636" t="s">
+        <v>631</v>
+      </c>
+      <c r="B636" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="637" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A637" t="s">
+        <v>632</v>
+      </c>
+      <c r="B637" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="638" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A638" t="s">
+        <v>633</v>
+      </c>
+      <c r="B638" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="639" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A639" t="s">
+        <v>634</v>
+      </c>
+      <c r="B639" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="640" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A640" t="s">
+        <v>635</v>
+      </c>
+      <c r="B640" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="641" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A641" t="s">
+        <v>636</v>
+      </c>
+      <c r="B641" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="642" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A642" t="s">
+        <v>637</v>
+      </c>
+      <c r="B642" t="s">
+        <v>518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>